<commit_message>
Update Site Web VueJS3
</commit_message>
<xml_diff>
--- a/Template/Data/Config_REFC.xlsx
+++ b/Template/Data/Config_REFC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renau\GitHub\RPA_Template-RHENRY\Template\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62450869-555B-435D-BA00-B17753DF0F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDA6938-435D-43D0-9195-6D021BF5C746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -216,9 +216,6 @@
     <t>Obligatoire</t>
   </si>
   <si>
-    <t>Identifiant</t>
-  </si>
-  <si>
     <t>CONFIG</t>
   </si>
   <si>
@@ -237,18 +234,12 @@
     <t>Email_ServeurSMTP</t>
   </si>
   <si>
-    <t>Email_CredentialSMTP</t>
-  </si>
-  <si>
     <t>Entier</t>
   </si>
   <si>
     <t>Port</t>
   </si>
   <si>
-    <t>LogDB_NOSQL_Credential</t>
-  </si>
-  <si>
     <t>Credential</t>
   </si>
   <si>
@@ -358,6 +349,24 @@
   </si>
   <si>
     <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Email_CredentialSMTP_Login</t>
+  </si>
+  <si>
+    <t>Pwd</t>
+  </si>
+  <si>
+    <t>Email_CredentialSMTP_Pwd</t>
+  </si>
+  <si>
+    <t>LogDB_NOSQL_Credential_Login</t>
+  </si>
+  <si>
+    <t>LogDB_NOSQL_Credential_Pwd</t>
   </si>
 </sst>
 </file>
@@ -5038,7 +5047,7 @@
         <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D2" s="5"/>
     </row>
@@ -5056,32 +5065,32 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
         <v>75</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C7" t="str">
         <f>C3&amp;"_"&amp;C2</f>
@@ -5090,10 +5099,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5101,7 +5110,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C10" t="str">
         <f>C3&amp;"_QueueName"</f>
@@ -5117,7 +5126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -5168,7 +5177,7 @@
     </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -5182,16 +5191,16 @@
     </row>
     <row r="3" spans="1:26" ht="30">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -5373,13 +5382,13 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -5390,18 +5399,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="26" width="65.42578125" customWidth="1"/>
   </cols>
@@ -5417,7 +5426,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
@@ -5454,13 +5463,13 @@
         <v>52</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>58</v>
@@ -5474,13 +5483,13 @@
         <v>55</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>58</v>
@@ -5494,13 +5503,13 @@
         <v>56</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>58</v>
@@ -5511,16 +5520,16 @@
         <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>58</v>
@@ -5536,19 +5545,19 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>58</v>
@@ -5556,19 +5565,19 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>58</v>
@@ -5576,60 +5585,60 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>67</v>
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
+        <v>106</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" t="s">
-        <v>54</v>
+      <c r="F10" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>53</v>
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
         <v>54</v>
@@ -5637,151 +5646,189 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>81</v>
+        <v>109</v>
+      </c>
+      <c r="D13" t="s">
+        <v>106</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" t="s">
-        <v>54</v>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:6" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="14.25" customHeight="1">
-      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
+        <v>59</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:6" ht="14.25" customHeight="1"/>
@@ -6755,10 +6802,12 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9 D12:D13 D15:D16 D2:D7 D18:D19 D21:D22" xr:uid="{EAD0B869-C39C-4665-BB02-4D2BB2300FFD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10 D14:D15 D17:D18 D23:D24 D20:D21 D2:D7" xr:uid="{EAD0B869-C39C-4665-BB02-4D2BB2300FFD}">
       <formula1>"Texte,Bool,Entier"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Init Settings OK ?
</commit_message>
<xml_diff>
--- a/Template/Data/Config_REFC.xlsx
+++ b/Template/Data/Config_REFC.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renau\GitHub\RPA_Template-RHENRY\Template\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58F70FD-D2D5-4EFD-85A0-35885E1A68B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E71133-BD7A-4528-9F54-FB36FF4D5517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV" sheetId="6" r:id="rId1"/>
     <sheet name="UAT" sheetId="5" r:id="rId2"/>
     <sheet name="PrePROD" sheetId="4" r:id="rId3"/>
     <sheet name="PROD" sheetId="1" r:id="rId4"/>
-    <sheet name="Core-Constante" sheetId="7" r:id="rId5"/>
-    <sheet name="Core-Assets" sheetId="8" r:id="rId6"/>
+    <sheet name="Core-Constants" sheetId="7" r:id="rId5"/>
+    <sheet name="Str" sheetId="8" r:id="rId6"/>
     <sheet name="Constants" sheetId="2" r:id="rId7"/>
     <sheet name="Assets" sheetId="3" r:id="rId8"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -380,12 +380,6 @@
   </si>
   <si>
     <t>Europe</t>
-  </si>
-  <si>
-    <t>Env</t>
-  </si>
-  <si>
-    <t>Environnement</t>
   </si>
   <si>
     <t>Performer</t>
@@ -885,10 +879,10 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="12">
         <v>2</v>
@@ -897,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -1966,10 +1960,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -1978,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -3047,10 +3041,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -3059,7 +3053,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -4127,10 +4121,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -4139,7 +4133,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -5245,10 +5239,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BC9249-B8A7-4BE9-B73B-28D49C06D735}">
-  <dimension ref="A1:AA983"/>
+  <dimension ref="A1:AA981"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D2" sqref="D2:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5309,13 +5303,13 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>52</v>
@@ -5324,93 +5318,48 @@
         <v>58</v>
       </c>
       <c r="F2" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
+      <c r="A3" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="9">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>57</v>
-      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>52</v>
@@ -5426,41 +5375,38 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1">
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A7" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="9">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
+    <row r="7" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:27" ht="14.25" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>52</v>
@@ -5468,1036 +5414,1012 @@
       <c r="E8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A10" s="7" t="s">
+    <row r="9" spans="1:27" ht="14.25" customHeight="1">
+      <c r="A9" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="B9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="17" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="18" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="19" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="20" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="21" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="22" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="23" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="24" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="25" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="26" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="27" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="28" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="29" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="30" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="31" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="32" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="33" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="34" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="35" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="36" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="37" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="38" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="39" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="40" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="41" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="42" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="43" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="44" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="45" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="46" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="47" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="48" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="49" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="50" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="51" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="52" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="53" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="54" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="55" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="56" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="57" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="58" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="59" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="60" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="61" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="62" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="63" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="64" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="65" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="66" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="67" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="68" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="69" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="70" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="71" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="72" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="73" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="74" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="75" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="76" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="77" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="78" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="79" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="80" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="81" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="82" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="83" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="84" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="85" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="86" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="87" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="88" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="89" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="90" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="91" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="92" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="93" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="94" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="95" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="96" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="97" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="98" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="99" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="100" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="101" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="102" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="103" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="104" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="105" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="106" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="107" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="108" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="109" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="110" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="111" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="112" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="113" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="114" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="115" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="116" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="117" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="118" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="119" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="120" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="121" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="122" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="123" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="124" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="125" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="126" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="127" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="128" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="129" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="130" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="131" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="132" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="133" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="134" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="135" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="136" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="137" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="138" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="139" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="140" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="141" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="142" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="143" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="144" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="145" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="146" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="147" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="148" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="149" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="150" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="151" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="152" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="153" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="154" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="155" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="156" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="157" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="158" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="159" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="160" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="161" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="162" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="163" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="164" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="165" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="166" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="167" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="168" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="169" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="170" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="171" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="172" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="173" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="174" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="175" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="176" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="177" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="178" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="179" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="180" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="181" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="182" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="183" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="184" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="185" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="186" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="187" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="188" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="189" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="190" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="191" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="192" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="193" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="194" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="195" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="196" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="197" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="198" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="199" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="200" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="201" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="202" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="203" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="204" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="205" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="206" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="207" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="208" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="209" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="210" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="211" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="212" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="213" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="214" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="215" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="216" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="217" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="218" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="219" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="220" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="221" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="222" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="223" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="224" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="225" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="226" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="227" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="228" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="229" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="230" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="231" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="232" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="233" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="234" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="235" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="236" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="237" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="238" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="239" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="240" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="241" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="242" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="243" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="244" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="245" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="246" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="247" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="248" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="249" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="250" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="251" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="252" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="253" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="254" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="255" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="256" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="257" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="258" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="259" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="260" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="261" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="262" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="263" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="264" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="265" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="266" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="267" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="268" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="269" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="270" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="271" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="272" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="273" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="274" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="275" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="276" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="277" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="278" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="279" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="280" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="281" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="282" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="283" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="284" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="285" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="286" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="287" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="288" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="289" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="290" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="291" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="292" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="293" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="294" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="295" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="296" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="297" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="298" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="299" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="300" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="301" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="302" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="303" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="304" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="305" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="306" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="307" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="308" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="309" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="310" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="311" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="312" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="313" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="314" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="315" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="316" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="317" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="318" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="319" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="320" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="321" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="322" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="323" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="324" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="325" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="326" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="327" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="328" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="329" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="330" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="331" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="332" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="333" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="334" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="335" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="336" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="337" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="338" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="339" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="340" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="341" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="342" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="343" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="344" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="345" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="346" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="347" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="348" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="349" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="350" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="351" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="352" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="353" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="354" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="355" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="356" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="357" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="358" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="359" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="360" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="361" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="362" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="363" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="364" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="365" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="366" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="367" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="368" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="369" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="370" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="371" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="372" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="373" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="374" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="375" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="376" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="377" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="378" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="379" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="380" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="381" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="382" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="383" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="384" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="385" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="386" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="387" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="388" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="389" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="390" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="391" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="392" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="393" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="394" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="395" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="396" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="397" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="398" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="399" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="400" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="401" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="402" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="403" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="404" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="405" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="406" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="407" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="408" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="409" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="410" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="411" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="412" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="413" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="414" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="415" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="416" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="417" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="418" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="419" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="420" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="421" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="422" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="423" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="424" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="425" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="426" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="427" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="428" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="429" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="430" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="431" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="432" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="433" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="434" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="435" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="436" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="437" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="438" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="439" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="440" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="441" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="442" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="443" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="444" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="445" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="446" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="447" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="448" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="449" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="450" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="451" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="452" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="453" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="454" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="455" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="456" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="457" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="458" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="459" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="460" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="461" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="462" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="463" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="464" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="465" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="466" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="467" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="468" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="469" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="470" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="471" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="472" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="473" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="474" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="475" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="476" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="477" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="478" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="479" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="480" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="481" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="482" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="483" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="484" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="485" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="486" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="487" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="488" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="489" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="490" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="491" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="492" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="493" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="494" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="495" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="496" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="497" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="498" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="499" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="500" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="501" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="502" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="503" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="504" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="505" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="506" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="507" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="508" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="509" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="510" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="511" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="512" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="513" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="514" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="515" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="516" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="517" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="518" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="519" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="520" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="521" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="522" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="523" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="524" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="525" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="526" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="527" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="528" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="529" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="530" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="531" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="532" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="533" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="534" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="535" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="536" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="537" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="538" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="539" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="540" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="541" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="542" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="543" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="544" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="545" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="546" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="547" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="548" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="549" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="550" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="551" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="552" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="553" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="554" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="555" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="556" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="557" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="558" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="559" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="560" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="561" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="562" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="563" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="564" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="565" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="566" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="567" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="568" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="569" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="570" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="571" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="572" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="573" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="574" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="575" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="576" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="577" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="578" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="579" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="580" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="581" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="582" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="583" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="584" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="585" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="586" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="587" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="588" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="589" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="590" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="591" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="592" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="593" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="594" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="595" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="596" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="597" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="598" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="599" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="600" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="601" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="602" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="603" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="604" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="605" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="606" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="607" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="608" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="609" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="610" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="611" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="612" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="613" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="614" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="615" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="616" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="617" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="618" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="619" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="620" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="621" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="622" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="623" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="624" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="625" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="626" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="627" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="628" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="629" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="630" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="631" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="632" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="633" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="634" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="635" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="636" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="637" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="638" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="639" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="640" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="641" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="642" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="643" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="644" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="645" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="646" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="647" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="648" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="649" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="650" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="651" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="652" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="653" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="654" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="655" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="656" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="657" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="658" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="659" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="660" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="661" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="662" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="663" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="664" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="665" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="666" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="667" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="668" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="669" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="670" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="671" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="672" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="673" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="674" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="675" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="676" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="677" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="678" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="679" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="680" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="681" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="682" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="683" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="684" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="685" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="686" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="687" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="688" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="689" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="690" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="691" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="692" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="693" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="694" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="695" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="696" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="697" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="698" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="699" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="700" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="701" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="702" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="703" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="704" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="705" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="706" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="707" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="708" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="709" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="710" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="711" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="712" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="713" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="714" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="715" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="716" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="717" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="718" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="719" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="720" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="721" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="722" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="723" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="724" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="725" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="726" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="727" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="728" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="729" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="730" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="731" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="732" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="733" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="734" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="735" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="736" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="737" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="738" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="739" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="740" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="741" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="742" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="743" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="744" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="745" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="746" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="747" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="748" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="749" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="750" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="751" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="752" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="753" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="754" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="755" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="756" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="757" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="758" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="759" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="760" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="761" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="762" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="763" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="764" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="765" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="766" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="767" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="768" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="769" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="770" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="771" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="772" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="773" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="774" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="775" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="776" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="777" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="778" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="779" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="780" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="781" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="782" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="783" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="784" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="785" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="786" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="787" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="788" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="789" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="790" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="791" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="792" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="793" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="794" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="795" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="796" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="797" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="798" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="799" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="800" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="801" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="802" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="803" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="804" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="805" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="806" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="807" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="808" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="809" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="810" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="811" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="812" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="813" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="814" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="815" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="816" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="817" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="818" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="819" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="820" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="821" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="822" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="823" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="824" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="825" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="826" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="827" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="828" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="829" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="830" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="831" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="832" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="833" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="834" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="835" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="836" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="837" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="838" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="839" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="840" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="841" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="842" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="843" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="844" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="845" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="846" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="847" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="848" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="849" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="850" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="851" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="852" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="853" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="854" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="855" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="856" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="857" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="858" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="859" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="860" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="861" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="862" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="863" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="864" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="865" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="866" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="867" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="868" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="869" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="870" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="871" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="872" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="873" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="874" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="875" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="876" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="877" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="878" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="879" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="880" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="881" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="882" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="883" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="884" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="885" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="886" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="887" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="888" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="889" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="890" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="891" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="892" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="893" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="894" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="895" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="896" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="897" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="898" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="899" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="900" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="901" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="902" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="903" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="904" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="905" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="906" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="907" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="908" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="909" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="910" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="911" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="912" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="913" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="914" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="915" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="916" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="917" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="918" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="919" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="920" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="921" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="922" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="923" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="924" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="925" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="926" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="927" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="928" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="929" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="930" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="931" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="932" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="933" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="934" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="935" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="936" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="937" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="938" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="939" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="940" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="941" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="942" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="943" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="944" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="945" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="946" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="947" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="948" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="949" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="950" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="951" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="952" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="953" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="954" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="955" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="956" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="957" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="958" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="959" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="960" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="961" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="962" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="963" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="964" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="965" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="966" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="967" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="968" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="969" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="970" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="971" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="972" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="973" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="974" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="975" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="976" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="977" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="978" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="979" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="980" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="981" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="982" s="7" customFormat="1" ht="14.25" customHeight="1"/>
-    <row r="983" s="7" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
+    <row r="115" ht="14.25" customHeight="1"/>
+    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="117" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1"/>
+    <row r="119" ht="14.25" customHeight="1"/>
+    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="121" ht="14.25" customHeight="1"/>
+    <row r="122" ht="14.25" customHeight="1"/>
+    <row r="123" ht="14.25" customHeight="1"/>
+    <row r="124" ht="14.25" customHeight="1"/>
+    <row r="125" ht="14.25" customHeight="1"/>
+    <row r="126" ht="14.25" customHeight="1"/>
+    <row r="127" ht="14.25" customHeight="1"/>
+    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="129" ht="14.25" customHeight="1"/>
+    <row r="130" ht="14.25" customHeight="1"/>
+    <row r="131" ht="14.25" customHeight="1"/>
+    <row r="132" ht="14.25" customHeight="1"/>
+    <row r="133" ht="14.25" customHeight="1"/>
+    <row r="134" ht="14.25" customHeight="1"/>
+    <row r="135" ht="14.25" customHeight="1"/>
+    <row r="136" ht="14.25" customHeight="1"/>
+    <row r="137" ht="14.25" customHeight="1"/>
+    <row r="138" ht="14.25" customHeight="1"/>
+    <row r="139" ht="14.25" customHeight="1"/>
+    <row r="140" ht="14.25" customHeight="1"/>
+    <row r="141" ht="14.25" customHeight="1"/>
+    <row r="142" ht="14.25" customHeight="1"/>
+    <row r="143" ht="14.25" customHeight="1"/>
+    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="145" ht="14.25" customHeight="1"/>
+    <row r="146" ht="14.25" customHeight="1"/>
+    <row r="147" ht="14.25" customHeight="1"/>
+    <row r="148" ht="14.25" customHeight="1"/>
+    <row r="149" ht="14.25" customHeight="1"/>
+    <row r="150" ht="14.25" customHeight="1"/>
+    <row r="151" ht="14.25" customHeight="1"/>
+    <row r="152" ht="14.25" customHeight="1"/>
+    <row r="153" ht="14.25" customHeight="1"/>
+    <row r="154" ht="14.25" customHeight="1"/>
+    <row r="155" ht="14.25" customHeight="1"/>
+    <row r="156" ht="14.25" customHeight="1"/>
+    <row r="157" ht="14.25" customHeight="1"/>
+    <row r="158" ht="14.25" customHeight="1"/>
+    <row r="159" ht="14.25" customHeight="1"/>
+    <row r="160" ht="14.25" customHeight="1"/>
+    <row r="161" ht="14.25" customHeight="1"/>
+    <row r="162" ht="14.25" customHeight="1"/>
+    <row r="163" ht="14.25" customHeight="1"/>
+    <row r="164" ht="14.25" customHeight="1"/>
+    <row r="165" ht="14.25" customHeight="1"/>
+    <row r="166" ht="14.25" customHeight="1"/>
+    <row r="167" ht="14.25" customHeight="1"/>
+    <row r="168" ht="14.25" customHeight="1"/>
+    <row r="169" ht="14.25" customHeight="1"/>
+    <row r="170" ht="14.25" customHeight="1"/>
+    <row r="171" ht="14.25" customHeight="1"/>
+    <row r="172" ht="14.25" customHeight="1"/>
+    <row r="173" ht="14.25" customHeight="1"/>
+    <row r="174" ht="14.25" customHeight="1"/>
+    <row r="175" ht="14.25" customHeight="1"/>
+    <row r="176" ht="14.25" customHeight="1"/>
+    <row r="177" ht="14.25" customHeight="1"/>
+    <row r="178" ht="14.25" customHeight="1"/>
+    <row r="179" ht="14.25" customHeight="1"/>
+    <row r="180" ht="14.25" customHeight="1"/>
+    <row r="181" ht="14.25" customHeight="1"/>
+    <row r="182" ht="14.25" customHeight="1"/>
+    <row r="183" ht="14.25" customHeight="1"/>
+    <row r="184" ht="14.25" customHeight="1"/>
+    <row r="185" ht="14.25" customHeight="1"/>
+    <row r="186" ht="14.25" customHeight="1"/>
+    <row r="187" ht="14.25" customHeight="1"/>
+    <row r="188" ht="14.25" customHeight="1"/>
+    <row r="189" ht="14.25" customHeight="1"/>
+    <row r="190" ht="14.25" customHeight="1"/>
+    <row r="191" ht="14.25" customHeight="1"/>
+    <row r="192" ht="14.25" customHeight="1"/>
+    <row r="193" ht="14.25" customHeight="1"/>
+    <row r="194" ht="14.25" customHeight="1"/>
+    <row r="195" ht="14.25" customHeight="1"/>
+    <row r="196" ht="14.25" customHeight="1"/>
+    <row r="197" ht="14.25" customHeight="1"/>
+    <row r="198" ht="14.25" customHeight="1"/>
+    <row r="199" ht="14.25" customHeight="1"/>
+    <row r="200" ht="14.25" customHeight="1"/>
+    <row r="201" ht="14.25" customHeight="1"/>
+    <row r="202" ht="14.25" customHeight="1"/>
+    <row r="203" ht="14.25" customHeight="1"/>
+    <row r="204" ht="14.25" customHeight="1"/>
+    <row r="205" ht="14.25" customHeight="1"/>
+    <row r="206" ht="14.25" customHeight="1"/>
+    <row r="207" ht="14.25" customHeight="1"/>
+    <row r="208" ht="14.25" customHeight="1"/>
+    <row r="209" ht="14.25" customHeight="1"/>
+    <row r="210" ht="14.25" customHeight="1"/>
+    <row r="211" ht="14.25" customHeight="1"/>
+    <row r="212" ht="14.25" customHeight="1"/>
+    <row r="213" ht="14.25" customHeight="1"/>
+    <row r="214" ht="14.25" customHeight="1"/>
+    <row r="215" ht="14.25" customHeight="1"/>
+    <row r="216" ht="14.25" customHeight="1"/>
+    <row r="217" ht="14.25" customHeight="1"/>
+    <row r="218" ht="14.25" customHeight="1"/>
+    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="220" ht="14.25" customHeight="1"/>
+    <row r="221" ht="14.25" customHeight="1"/>
+    <row r="222" ht="14.25" customHeight="1"/>
+    <row r="223" ht="14.25" customHeight="1"/>
+    <row r="224" ht="14.25" customHeight="1"/>
+    <row r="225" ht="14.25" customHeight="1"/>
+    <row r="226" ht="14.25" customHeight="1"/>
+    <row r="227" ht="14.25" customHeight="1"/>
+    <row r="228" ht="14.25" customHeight="1"/>
+    <row r="229" ht="14.25" customHeight="1"/>
+    <row r="230" ht="14.25" customHeight="1"/>
+    <row r="231" ht="14.25" customHeight="1"/>
+    <row r="232" ht="14.25" customHeight="1"/>
+    <row r="233" ht="14.25" customHeight="1"/>
+    <row r="234" ht="14.25" customHeight="1"/>
+    <row r="235" ht="14.25" customHeight="1"/>
+    <row r="236" ht="14.25" customHeight="1"/>
+    <row r="237" ht="14.25" customHeight="1"/>
+    <row r="238" ht="14.25" customHeight="1"/>
+    <row r="239" ht="14.25" customHeight="1"/>
+    <row r="240" ht="14.25" customHeight="1"/>
+    <row r="241" ht="14.25" customHeight="1"/>
+    <row r="242" ht="14.25" customHeight="1"/>
+    <row r="243" ht="14.25" customHeight="1"/>
+    <row r="244" ht="14.25" customHeight="1"/>
+    <row r="245" ht="14.25" customHeight="1"/>
+    <row r="246" ht="14.25" customHeight="1"/>
+    <row r="247" ht="14.25" customHeight="1"/>
+    <row r="248" ht="14.25" customHeight="1"/>
+    <row r="249" ht="14.25" customHeight="1"/>
+    <row r="250" ht="14.25" customHeight="1"/>
+    <row r="251" ht="14.25" customHeight="1"/>
+    <row r="252" ht="14.25" customHeight="1"/>
+    <row r="253" ht="14.25" customHeight="1"/>
+    <row r="254" ht="14.25" customHeight="1"/>
+    <row r="255" ht="14.25" customHeight="1"/>
+    <row r="256" ht="14.25" customHeight="1"/>
+    <row r="257" ht="14.25" customHeight="1"/>
+    <row r="258" ht="14.25" customHeight="1"/>
+    <row r="259" ht="14.25" customHeight="1"/>
+    <row r="260" ht="14.25" customHeight="1"/>
+    <row r="261" ht="14.25" customHeight="1"/>
+    <row r="262" ht="14.25" customHeight="1"/>
+    <row r="263" ht="14.25" customHeight="1"/>
+    <row r="264" ht="14.25" customHeight="1"/>
+    <row r="265" ht="14.25" customHeight="1"/>
+    <row r="266" ht="14.25" customHeight="1"/>
+    <row r="267" ht="14.25" customHeight="1"/>
+    <row r="268" ht="14.25" customHeight="1"/>
+    <row r="269" ht="14.25" customHeight="1"/>
+    <row r="270" ht="14.25" customHeight="1"/>
+    <row r="271" ht="14.25" customHeight="1"/>
+    <row r="272" ht="14.25" customHeight="1"/>
+    <row r="273" ht="14.25" customHeight="1"/>
+    <row r="274" ht="14.25" customHeight="1"/>
+    <row r="275" ht="14.25" customHeight="1"/>
+    <row r="276" ht="14.25" customHeight="1"/>
+    <row r="277" ht="14.25" customHeight="1"/>
+    <row r="278" ht="14.25" customHeight="1"/>
+    <row r="279" ht="14.25" customHeight="1"/>
+    <row r="280" ht="14.25" customHeight="1"/>
+    <row r="281" ht="14.25" customHeight="1"/>
+    <row r="282" ht="14.25" customHeight="1"/>
+    <row r="283" ht="14.25" customHeight="1"/>
+    <row r="284" ht="14.25" customHeight="1"/>
+    <row r="285" ht="14.25" customHeight="1"/>
+    <row r="286" ht="14.25" customHeight="1"/>
+    <row r="287" ht="14.25" customHeight="1"/>
+    <row r="288" ht="14.25" customHeight="1"/>
+    <row r="289" ht="14.25" customHeight="1"/>
+    <row r="290" ht="14.25" customHeight="1"/>
+    <row r="291" ht="14.25" customHeight="1"/>
+    <row r="292" ht="14.25" customHeight="1"/>
+    <row r="293" ht="14.25" customHeight="1"/>
+    <row r="294" ht="14.25" customHeight="1"/>
+    <row r="295" ht="14.25" customHeight="1"/>
+    <row r="296" ht="14.25" customHeight="1"/>
+    <row r="297" ht="14.25" customHeight="1"/>
+    <row r="298" ht="14.25" customHeight="1"/>
+    <row r="299" ht="14.25" customHeight="1"/>
+    <row r="300" ht="14.25" customHeight="1"/>
+    <row r="301" ht="14.25" customHeight="1"/>
+    <row r="302" ht="14.25" customHeight="1"/>
+    <row r="303" ht="14.25" customHeight="1"/>
+    <row r="304" ht="14.25" customHeight="1"/>
+    <row r="305" ht="14.25" customHeight="1"/>
+    <row r="306" ht="14.25" customHeight="1"/>
+    <row r="307" ht="14.25" customHeight="1"/>
+    <row r="308" ht="14.25" customHeight="1"/>
+    <row r="309" ht="14.25" customHeight="1"/>
+    <row r="310" ht="14.25" customHeight="1"/>
+    <row r="311" ht="14.25" customHeight="1"/>
+    <row r="312" ht="14.25" customHeight="1"/>
+    <row r="313" ht="14.25" customHeight="1"/>
+    <row r="314" ht="14.25" customHeight="1"/>
+    <row r="315" ht="14.25" customHeight="1"/>
+    <row r="316" ht="14.25" customHeight="1"/>
+    <row r="317" ht="14.25" customHeight="1"/>
+    <row r="318" ht="14.25" customHeight="1"/>
+    <row r="319" ht="14.25" customHeight="1"/>
+    <row r="320" ht="14.25" customHeight="1"/>
+    <row r="321" ht="14.25" customHeight="1"/>
+    <row r="322" ht="14.25" customHeight="1"/>
+    <row r="323" ht="14.25" customHeight="1"/>
+    <row r="324" ht="14.25" customHeight="1"/>
+    <row r="325" ht="14.25" customHeight="1"/>
+    <row r="326" ht="14.25" customHeight="1"/>
+    <row r="327" ht="14.25" customHeight="1"/>
+    <row r="328" ht="14.25" customHeight="1"/>
+    <row r="329" ht="14.25" customHeight="1"/>
+    <row r="330" ht="14.25" customHeight="1"/>
+    <row r="331" ht="14.25" customHeight="1"/>
+    <row r="332" ht="14.25" customHeight="1"/>
+    <row r="333" ht="14.25" customHeight="1"/>
+    <row r="334" ht="14.25" customHeight="1"/>
+    <row r="335" ht="14.25" customHeight="1"/>
+    <row r="336" ht="14.25" customHeight="1"/>
+    <row r="337" ht="14.25" customHeight="1"/>
+    <row r="338" ht="14.25" customHeight="1"/>
+    <row r="339" ht="14.25" customHeight="1"/>
+    <row r="340" ht="14.25" customHeight="1"/>
+    <row r="341" ht="14.25" customHeight="1"/>
+    <row r="342" ht="14.25" customHeight="1"/>
+    <row r="343" ht="14.25" customHeight="1"/>
+    <row r="344" ht="14.25" customHeight="1"/>
+    <row r="345" ht="14.25" customHeight="1"/>
+    <row r="346" ht="14.25" customHeight="1"/>
+    <row r="347" ht="14.25" customHeight="1"/>
+    <row r="348" ht="14.25" customHeight="1"/>
+    <row r="349" ht="14.25" customHeight="1"/>
+    <row r="350" ht="14.25" customHeight="1"/>
+    <row r="351" ht="14.25" customHeight="1"/>
+    <row r="352" ht="14.25" customHeight="1"/>
+    <row r="353" ht="14.25" customHeight="1"/>
+    <row r="354" ht="14.25" customHeight="1"/>
+    <row r="355" ht="14.25" customHeight="1"/>
+    <row r="356" ht="14.25" customHeight="1"/>
+    <row r="357" ht="14.25" customHeight="1"/>
+    <row r="358" ht="14.25" customHeight="1"/>
+    <row r="359" ht="14.25" customHeight="1"/>
+    <row r="360" ht="14.25" customHeight="1"/>
+    <row r="361" ht="14.25" customHeight="1"/>
+    <row r="362" ht="14.25" customHeight="1"/>
+    <row r="363" ht="14.25" customHeight="1"/>
+    <row r="364" ht="14.25" customHeight="1"/>
+    <row r="365" ht="14.25" customHeight="1"/>
+    <row r="366" ht="14.25" customHeight="1"/>
+    <row r="367" ht="14.25" customHeight="1"/>
+    <row r="368" ht="14.25" customHeight="1"/>
+    <row r="369" ht="14.25" customHeight="1"/>
+    <row r="370" ht="14.25" customHeight="1"/>
+    <row r="371" ht="14.25" customHeight="1"/>
+    <row r="372" ht="14.25" customHeight="1"/>
+    <row r="373" ht="14.25" customHeight="1"/>
+    <row r="374" ht="14.25" customHeight="1"/>
+    <row r="375" ht="14.25" customHeight="1"/>
+    <row r="376" ht="14.25" customHeight="1"/>
+    <row r="377" ht="14.25" customHeight="1"/>
+    <row r="378" ht="14.25" customHeight="1"/>
+    <row r="379" ht="14.25" customHeight="1"/>
+    <row r="380" ht="14.25" customHeight="1"/>
+    <row r="381" ht="14.25" customHeight="1"/>
+    <row r="382" ht="14.25" customHeight="1"/>
+    <row r="383" ht="14.25" customHeight="1"/>
+    <row r="384" ht="14.25" customHeight="1"/>
+    <row r="385" ht="14.25" customHeight="1"/>
+    <row r="386" ht="14.25" customHeight="1"/>
+    <row r="387" ht="14.25" customHeight="1"/>
+    <row r="388" ht="14.25" customHeight="1"/>
+    <row r="389" ht="14.25" customHeight="1"/>
+    <row r="390" ht="14.25" customHeight="1"/>
+    <row r="391" ht="14.25" customHeight="1"/>
+    <row r="392" ht="14.25" customHeight="1"/>
+    <row r="393" ht="14.25" customHeight="1"/>
+    <row r="394" ht="14.25" customHeight="1"/>
+    <row r="395" ht="14.25" customHeight="1"/>
+    <row r="396" ht="14.25" customHeight="1"/>
+    <row r="397" ht="14.25" customHeight="1"/>
+    <row r="398" ht="14.25" customHeight="1"/>
+    <row r="399" ht="14.25" customHeight="1"/>
+    <row r="400" ht="14.25" customHeight="1"/>
+    <row r="401" ht="14.25" customHeight="1"/>
+    <row r="402" ht="14.25" customHeight="1"/>
+    <row r="403" ht="14.25" customHeight="1"/>
+    <row r="404" ht="14.25" customHeight="1"/>
+    <row r="405" ht="14.25" customHeight="1"/>
+    <row r="406" ht="14.25" customHeight="1"/>
+    <row r="407" ht="14.25" customHeight="1"/>
+    <row r="408" ht="14.25" customHeight="1"/>
+    <row r="409" ht="14.25" customHeight="1"/>
+    <row r="410" ht="14.25" customHeight="1"/>
+    <row r="411" ht="14.25" customHeight="1"/>
+    <row r="412" ht="14.25" customHeight="1"/>
+    <row r="413" ht="14.25" customHeight="1"/>
+    <row r="414" ht="14.25" customHeight="1"/>
+    <row r="415" ht="14.25" customHeight="1"/>
+    <row r="416" ht="14.25" customHeight="1"/>
+    <row r="417" ht="14.25" customHeight="1"/>
+    <row r="418" ht="14.25" customHeight="1"/>
+    <row r="419" ht="14.25" customHeight="1"/>
+    <row r="420" ht="14.25" customHeight="1"/>
+    <row r="421" ht="14.25" customHeight="1"/>
+    <row r="422" ht="14.25" customHeight="1"/>
+    <row r="423" ht="14.25" customHeight="1"/>
+    <row r="424" ht="14.25" customHeight="1"/>
+    <row r="425" ht="14.25" customHeight="1"/>
+    <row r="426" ht="14.25" customHeight="1"/>
+    <row r="427" ht="14.25" customHeight="1"/>
+    <row r="428" ht="14.25" customHeight="1"/>
+    <row r="429" ht="14.25" customHeight="1"/>
+    <row r="430" ht="14.25" customHeight="1"/>
+    <row r="431" ht="14.25" customHeight="1"/>
+    <row r="432" ht="14.25" customHeight="1"/>
+    <row r="433" ht="14.25" customHeight="1"/>
+    <row r="434" ht="14.25" customHeight="1"/>
+    <row r="435" ht="14.25" customHeight="1"/>
+    <row r="436" ht="14.25" customHeight="1"/>
+    <row r="437" ht="14.25" customHeight="1"/>
+    <row r="438" ht="14.25" customHeight="1"/>
+    <row r="439" ht="14.25" customHeight="1"/>
+    <row r="440" ht="14.25" customHeight="1"/>
+    <row r="441" ht="14.25" customHeight="1"/>
+    <row r="442" ht="14.25" customHeight="1"/>
+    <row r="443" ht="14.25" customHeight="1"/>
+    <row r="444" ht="14.25" customHeight="1"/>
+    <row r="445" ht="14.25" customHeight="1"/>
+    <row r="446" ht="14.25" customHeight="1"/>
+    <row r="447" ht="14.25" customHeight="1"/>
+    <row r="448" ht="14.25" customHeight="1"/>
+    <row r="449" ht="14.25" customHeight="1"/>
+    <row r="450" ht="14.25" customHeight="1"/>
+    <row r="451" ht="14.25" customHeight="1"/>
+    <row r="452" ht="14.25" customHeight="1"/>
+    <row r="453" ht="14.25" customHeight="1"/>
+    <row r="454" ht="14.25" customHeight="1"/>
+    <row r="455" ht="14.25" customHeight="1"/>
+    <row r="456" ht="14.25" customHeight="1"/>
+    <row r="457" ht="14.25" customHeight="1"/>
+    <row r="458" ht="14.25" customHeight="1"/>
+    <row r="459" ht="14.25" customHeight="1"/>
+    <row r="460" ht="14.25" customHeight="1"/>
+    <row r="461" ht="14.25" customHeight="1"/>
+    <row r="462" ht="14.25" customHeight="1"/>
+    <row r="463" ht="14.25" customHeight="1"/>
+    <row r="464" ht="14.25" customHeight="1"/>
+    <row r="465" ht="14.25" customHeight="1"/>
+    <row r="466" ht="14.25" customHeight="1"/>
+    <row r="467" ht="14.25" customHeight="1"/>
+    <row r="468" ht="14.25" customHeight="1"/>
+    <row r="469" ht="14.25" customHeight="1"/>
+    <row r="470" ht="14.25" customHeight="1"/>
+    <row r="471" ht="14.25" customHeight="1"/>
+    <row r="472" ht="14.25" customHeight="1"/>
+    <row r="473" ht="14.25" customHeight="1"/>
+    <row r="474" ht="14.25" customHeight="1"/>
+    <row r="475" ht="14.25" customHeight="1"/>
+    <row r="476" ht="14.25" customHeight="1"/>
+    <row r="477" ht="14.25" customHeight="1"/>
+    <row r="478" ht="14.25" customHeight="1"/>
+    <row r="479" ht="14.25" customHeight="1"/>
+    <row r="480" ht="14.25" customHeight="1"/>
+    <row r="481" ht="14.25" customHeight="1"/>
+    <row r="482" ht="14.25" customHeight="1"/>
+    <row r="483" ht="14.25" customHeight="1"/>
+    <row r="484" ht="14.25" customHeight="1"/>
+    <row r="485" ht="14.25" customHeight="1"/>
+    <row r="486" ht="14.25" customHeight="1"/>
+    <row r="487" ht="14.25" customHeight="1"/>
+    <row r="488" ht="14.25" customHeight="1"/>
+    <row r="489" ht="14.25" customHeight="1"/>
+    <row r="490" ht="14.25" customHeight="1"/>
+    <row r="491" ht="14.25" customHeight="1"/>
+    <row r="492" ht="14.25" customHeight="1"/>
+    <row r="493" ht="14.25" customHeight="1"/>
+    <row r="494" ht="14.25" customHeight="1"/>
+    <row r="495" ht="14.25" customHeight="1"/>
+    <row r="496" ht="14.25" customHeight="1"/>
+    <row r="497" ht="14.25" customHeight="1"/>
+    <row r="498" ht="14.25" customHeight="1"/>
+    <row r="499" ht="14.25" customHeight="1"/>
+    <row r="500" ht="14.25" customHeight="1"/>
+    <row r="501" ht="14.25" customHeight="1"/>
+    <row r="502" ht="14.25" customHeight="1"/>
+    <row r="503" ht="14.25" customHeight="1"/>
+    <row r="504" ht="14.25" customHeight="1"/>
+    <row r="505" ht="14.25" customHeight="1"/>
+    <row r="506" ht="14.25" customHeight="1"/>
+    <row r="507" ht="14.25" customHeight="1"/>
+    <row r="508" ht="14.25" customHeight="1"/>
+    <row r="509" ht="14.25" customHeight="1"/>
+    <row r="510" ht="14.25" customHeight="1"/>
+    <row r="511" ht="14.25" customHeight="1"/>
+    <row r="512" ht="14.25" customHeight="1"/>
+    <row r="513" ht="14.25" customHeight="1"/>
+    <row r="514" ht="14.25" customHeight="1"/>
+    <row r="515" ht="14.25" customHeight="1"/>
+    <row r="516" ht="14.25" customHeight="1"/>
+    <row r="517" ht="14.25" customHeight="1"/>
+    <row r="518" ht="14.25" customHeight="1"/>
+    <row r="519" ht="14.25" customHeight="1"/>
+    <row r="520" ht="14.25" customHeight="1"/>
+    <row r="521" ht="14.25" customHeight="1"/>
+    <row r="522" ht="14.25" customHeight="1"/>
+    <row r="523" ht="14.25" customHeight="1"/>
+    <row r="524" ht="14.25" customHeight="1"/>
+    <row r="525" ht="14.25" customHeight="1"/>
+    <row r="526" ht="14.25" customHeight="1"/>
+    <row r="527" ht="14.25" customHeight="1"/>
+    <row r="528" ht="14.25" customHeight="1"/>
+    <row r="529" ht="14.25" customHeight="1"/>
+    <row r="530" ht="14.25" customHeight="1"/>
+    <row r="531" ht="14.25" customHeight="1"/>
+    <row r="532" ht="14.25" customHeight="1"/>
+    <row r="533" ht="14.25" customHeight="1"/>
+    <row r="534" ht="14.25" customHeight="1"/>
+    <row r="535" ht="14.25" customHeight="1"/>
+    <row r="536" ht="14.25" customHeight="1"/>
+    <row r="537" ht="14.25" customHeight="1"/>
+    <row r="538" ht="14.25" customHeight="1"/>
+    <row r="539" ht="14.25" customHeight="1"/>
+    <row r="540" ht="14.25" customHeight="1"/>
+    <row r="541" ht="14.25" customHeight="1"/>
+    <row r="542" ht="14.25" customHeight="1"/>
+    <row r="543" ht="14.25" customHeight="1"/>
+    <row r="544" ht="14.25" customHeight="1"/>
+    <row r="545" ht="14.25" customHeight="1"/>
+    <row r="546" ht="14.25" customHeight="1"/>
+    <row r="547" ht="14.25" customHeight="1"/>
+    <row r="548" ht="14.25" customHeight="1"/>
+    <row r="549" ht="14.25" customHeight="1"/>
+    <row r="550" ht="14.25" customHeight="1"/>
+    <row r="551" ht="14.25" customHeight="1"/>
+    <row r="552" ht="14.25" customHeight="1"/>
+    <row r="553" ht="14.25" customHeight="1"/>
+    <row r="554" ht="14.25" customHeight="1"/>
+    <row r="555" ht="14.25" customHeight="1"/>
+    <row r="556" ht="14.25" customHeight="1"/>
+    <row r="557" ht="14.25" customHeight="1"/>
+    <row r="558" ht="14.25" customHeight="1"/>
+    <row r="559" ht="14.25" customHeight="1"/>
+    <row r="560" ht="14.25" customHeight="1"/>
+    <row r="561" ht="14.25" customHeight="1"/>
+    <row r="562" ht="14.25" customHeight="1"/>
+    <row r="563" ht="14.25" customHeight="1"/>
+    <row r="564" ht="14.25" customHeight="1"/>
+    <row r="565" ht="14.25" customHeight="1"/>
+    <row r="566" ht="14.25" customHeight="1"/>
+    <row r="567" ht="14.25" customHeight="1"/>
+    <row r="568" ht="14.25" customHeight="1"/>
+    <row r="569" ht="14.25" customHeight="1"/>
+    <row r="570" ht="14.25" customHeight="1"/>
+    <row r="571" ht="14.25" customHeight="1"/>
+    <row r="572" ht="14.25" customHeight="1"/>
+    <row r="573" ht="14.25" customHeight="1"/>
+    <row r="574" ht="14.25" customHeight="1"/>
+    <row r="575" ht="14.25" customHeight="1"/>
+    <row r="576" ht="14.25" customHeight="1"/>
+    <row r="577" ht="14.25" customHeight="1"/>
+    <row r="578" ht="14.25" customHeight="1"/>
+    <row r="579" ht="14.25" customHeight="1"/>
+    <row r="580" ht="14.25" customHeight="1"/>
+    <row r="581" ht="14.25" customHeight="1"/>
+    <row r="582" ht="14.25" customHeight="1"/>
+    <row r="583" ht="14.25" customHeight="1"/>
+    <row r="584" ht="14.25" customHeight="1"/>
+    <row r="585" ht="14.25" customHeight="1"/>
+    <row r="586" ht="14.25" customHeight="1"/>
+    <row r="587" ht="14.25" customHeight="1"/>
+    <row r="588" ht="14.25" customHeight="1"/>
+    <row r="589" ht="14.25" customHeight="1"/>
+    <row r="590" ht="14.25" customHeight="1"/>
+    <row r="591" ht="14.25" customHeight="1"/>
+    <row r="592" ht="14.25" customHeight="1"/>
+    <row r="593" ht="14.25" customHeight="1"/>
+    <row r="594" ht="14.25" customHeight="1"/>
+    <row r="595" ht="14.25" customHeight="1"/>
+    <row r="596" ht="14.25" customHeight="1"/>
+    <row r="597" ht="14.25" customHeight="1"/>
+    <row r="598" ht="14.25" customHeight="1"/>
+    <row r="599" ht="14.25" customHeight="1"/>
+    <row r="600" ht="14.25" customHeight="1"/>
+    <row r="601" ht="14.25" customHeight="1"/>
+    <row r="602" ht="14.25" customHeight="1"/>
+    <row r="603" ht="14.25" customHeight="1"/>
+    <row r="604" ht="14.25" customHeight="1"/>
+    <row r="605" ht="14.25" customHeight="1"/>
+    <row r="606" ht="14.25" customHeight="1"/>
+    <row r="607" ht="14.25" customHeight="1"/>
+    <row r="608" ht="14.25" customHeight="1"/>
+    <row r="609" ht="14.25" customHeight="1"/>
+    <row r="610" ht="14.25" customHeight="1"/>
+    <row r="611" ht="14.25" customHeight="1"/>
+    <row r="612" ht="14.25" customHeight="1"/>
+    <row r="613" ht="14.25" customHeight="1"/>
+    <row r="614" ht="14.25" customHeight="1"/>
+    <row r="615" ht="14.25" customHeight="1"/>
+    <row r="616" ht="14.25" customHeight="1"/>
+    <row r="617" ht="14.25" customHeight="1"/>
+    <row r="618" ht="14.25" customHeight="1"/>
+    <row r="619" ht="14.25" customHeight="1"/>
+    <row r="620" ht="14.25" customHeight="1"/>
+    <row r="621" ht="14.25" customHeight="1"/>
+    <row r="622" ht="14.25" customHeight="1"/>
+    <row r="623" ht="14.25" customHeight="1"/>
+    <row r="624" ht="14.25" customHeight="1"/>
+    <row r="625" ht="14.25" customHeight="1"/>
+    <row r="626" ht="14.25" customHeight="1"/>
+    <row r="627" ht="14.25" customHeight="1"/>
+    <row r="628" ht="14.25" customHeight="1"/>
+    <row r="629" ht="14.25" customHeight="1"/>
+    <row r="630" ht="14.25" customHeight="1"/>
+    <row r="631" ht="14.25" customHeight="1"/>
+    <row r="632" ht="14.25" customHeight="1"/>
+    <row r="633" ht="14.25" customHeight="1"/>
+    <row r="634" ht="14.25" customHeight="1"/>
+    <row r="635" ht="14.25" customHeight="1"/>
+    <row r="636" ht="14.25" customHeight="1"/>
+    <row r="637" ht="14.25" customHeight="1"/>
+    <row r="638" ht="14.25" customHeight="1"/>
+    <row r="639" ht="14.25" customHeight="1"/>
+    <row r="640" ht="14.25" customHeight="1"/>
+    <row r="641" ht="14.25" customHeight="1"/>
+    <row r="642" ht="14.25" customHeight="1"/>
+    <row r="643" ht="14.25" customHeight="1"/>
+    <row r="644" ht="14.25" customHeight="1"/>
+    <row r="645" ht="14.25" customHeight="1"/>
+    <row r="646" ht="14.25" customHeight="1"/>
+    <row r="647" ht="14.25" customHeight="1"/>
+    <row r="648" ht="14.25" customHeight="1"/>
+    <row r="649" ht="14.25" customHeight="1"/>
+    <row r="650" ht="14.25" customHeight="1"/>
+    <row r="651" ht="14.25" customHeight="1"/>
+    <row r="652" ht="14.25" customHeight="1"/>
+    <row r="653" ht="14.25" customHeight="1"/>
+    <row r="654" ht="14.25" customHeight="1"/>
+    <row r="655" ht="14.25" customHeight="1"/>
+    <row r="656" ht="14.25" customHeight="1"/>
+    <row r="657" ht="14.25" customHeight="1"/>
+    <row r="658" ht="14.25" customHeight="1"/>
+    <row r="659" ht="14.25" customHeight="1"/>
+    <row r="660" ht="14.25" customHeight="1"/>
+    <row r="661" ht="14.25" customHeight="1"/>
+    <row r="662" ht="14.25" customHeight="1"/>
+    <row r="663" ht="14.25" customHeight="1"/>
+    <row r="664" ht="14.25" customHeight="1"/>
+    <row r="665" ht="14.25" customHeight="1"/>
+    <row r="666" ht="14.25" customHeight="1"/>
+    <row r="667" ht="14.25" customHeight="1"/>
+    <row r="668" ht="14.25" customHeight="1"/>
+    <row r="669" ht="14.25" customHeight="1"/>
+    <row r="670" ht="14.25" customHeight="1"/>
+    <row r="671" ht="14.25" customHeight="1"/>
+    <row r="672" ht="14.25" customHeight="1"/>
+    <row r="673" ht="14.25" customHeight="1"/>
+    <row r="674" ht="14.25" customHeight="1"/>
+    <row r="675" ht="14.25" customHeight="1"/>
+    <row r="676" ht="14.25" customHeight="1"/>
+    <row r="677" ht="14.25" customHeight="1"/>
+    <row r="678" ht="14.25" customHeight="1"/>
+    <row r="679" ht="14.25" customHeight="1"/>
+    <row r="680" ht="14.25" customHeight="1"/>
+    <row r="681" ht="14.25" customHeight="1"/>
+    <row r="682" ht="14.25" customHeight="1"/>
+    <row r="683" ht="14.25" customHeight="1"/>
+    <row r="684" ht="14.25" customHeight="1"/>
+    <row r="685" ht="14.25" customHeight="1"/>
+    <row r="686" ht="14.25" customHeight="1"/>
+    <row r="687" ht="14.25" customHeight="1"/>
+    <row r="688" ht="14.25" customHeight="1"/>
+    <row r="689" ht="14.25" customHeight="1"/>
+    <row r="690" ht="14.25" customHeight="1"/>
+    <row r="691" ht="14.25" customHeight="1"/>
+    <row r="692" ht="14.25" customHeight="1"/>
+    <row r="693" ht="14.25" customHeight="1"/>
+    <row r="694" ht="14.25" customHeight="1"/>
+    <row r="695" ht="14.25" customHeight="1"/>
+    <row r="696" ht="14.25" customHeight="1"/>
+    <row r="697" ht="14.25" customHeight="1"/>
+    <row r="698" ht="14.25" customHeight="1"/>
+    <row r="699" ht="14.25" customHeight="1"/>
+    <row r="700" ht="14.25" customHeight="1"/>
+    <row r="701" ht="14.25" customHeight="1"/>
+    <row r="702" ht="14.25" customHeight="1"/>
+    <row r="703" ht="14.25" customHeight="1"/>
+    <row r="704" ht="14.25" customHeight="1"/>
+    <row r="705" ht="14.25" customHeight="1"/>
+    <row r="706" ht="14.25" customHeight="1"/>
+    <row r="707" ht="14.25" customHeight="1"/>
+    <row r="708" ht="14.25" customHeight="1"/>
+    <row r="709" ht="14.25" customHeight="1"/>
+    <row r="710" ht="14.25" customHeight="1"/>
+    <row r="711" ht="14.25" customHeight="1"/>
+    <row r="712" ht="14.25" customHeight="1"/>
+    <row r="713" ht="14.25" customHeight="1"/>
+    <row r="714" ht="14.25" customHeight="1"/>
+    <row r="715" ht="14.25" customHeight="1"/>
+    <row r="716" ht="14.25" customHeight="1"/>
+    <row r="717" ht="14.25" customHeight="1"/>
+    <row r="718" ht="14.25" customHeight="1"/>
+    <row r="719" ht="14.25" customHeight="1"/>
+    <row r="720" ht="14.25" customHeight="1"/>
+    <row r="721" ht="14.25" customHeight="1"/>
+    <row r="722" ht="14.25" customHeight="1"/>
+    <row r="723" ht="14.25" customHeight="1"/>
+    <row r="724" ht="14.25" customHeight="1"/>
+    <row r="725" ht="14.25" customHeight="1"/>
+    <row r="726" ht="14.25" customHeight="1"/>
+    <row r="727" ht="14.25" customHeight="1"/>
+    <row r="728" ht="14.25" customHeight="1"/>
+    <row r="729" ht="14.25" customHeight="1"/>
+    <row r="730" ht="14.25" customHeight="1"/>
+    <row r="731" ht="14.25" customHeight="1"/>
+    <row r="732" ht="14.25" customHeight="1"/>
+    <row r="733" ht="14.25" customHeight="1"/>
+    <row r="734" ht="14.25" customHeight="1"/>
+    <row r="735" ht="14.25" customHeight="1"/>
+    <row r="736" ht="14.25" customHeight="1"/>
+    <row r="737" ht="14.25" customHeight="1"/>
+    <row r="738" ht="14.25" customHeight="1"/>
+    <row r="739" ht="14.25" customHeight="1"/>
+    <row r="740" ht="14.25" customHeight="1"/>
+    <row r="741" ht="14.25" customHeight="1"/>
+    <row r="742" ht="14.25" customHeight="1"/>
+    <row r="743" ht="14.25" customHeight="1"/>
+    <row r="744" ht="14.25" customHeight="1"/>
+    <row r="745" ht="14.25" customHeight="1"/>
+    <row r="746" ht="14.25" customHeight="1"/>
+    <row r="747" ht="14.25" customHeight="1"/>
+    <row r="748" ht="14.25" customHeight="1"/>
+    <row r="749" ht="14.25" customHeight="1"/>
+    <row r="750" ht="14.25" customHeight="1"/>
+    <row r="751" ht="14.25" customHeight="1"/>
+    <row r="752" ht="14.25" customHeight="1"/>
+    <row r="753" ht="14.25" customHeight="1"/>
+    <row r="754" ht="14.25" customHeight="1"/>
+    <row r="755" ht="14.25" customHeight="1"/>
+    <row r="756" ht="14.25" customHeight="1"/>
+    <row r="757" ht="14.25" customHeight="1"/>
+    <row r="758" ht="14.25" customHeight="1"/>
+    <row r="759" ht="14.25" customHeight="1"/>
+    <row r="760" ht="14.25" customHeight="1"/>
+    <row r="761" ht="14.25" customHeight="1"/>
+    <row r="762" ht="14.25" customHeight="1"/>
+    <row r="763" ht="14.25" customHeight="1"/>
+    <row r="764" ht="14.25" customHeight="1"/>
+    <row r="765" ht="14.25" customHeight="1"/>
+    <row r="766" ht="14.25" customHeight="1"/>
+    <row r="767" ht="14.25" customHeight="1"/>
+    <row r="768" ht="14.25" customHeight="1"/>
+    <row r="769" ht="14.25" customHeight="1"/>
+    <row r="770" ht="14.25" customHeight="1"/>
+    <row r="771" ht="14.25" customHeight="1"/>
+    <row r="772" ht="14.25" customHeight="1"/>
+    <row r="773" ht="14.25" customHeight="1"/>
+    <row r="774" ht="14.25" customHeight="1"/>
+    <row r="775" ht="14.25" customHeight="1"/>
+    <row r="776" ht="14.25" customHeight="1"/>
+    <row r="777" ht="14.25" customHeight="1"/>
+    <row r="778" ht="14.25" customHeight="1"/>
+    <row r="779" ht="14.25" customHeight="1"/>
+    <row r="780" ht="14.25" customHeight="1"/>
+    <row r="781" ht="14.25" customHeight="1"/>
+    <row r="782" ht="14.25" customHeight="1"/>
+    <row r="783" ht="14.25" customHeight="1"/>
+    <row r="784" ht="14.25" customHeight="1"/>
+    <row r="785" ht="14.25" customHeight="1"/>
+    <row r="786" ht="14.25" customHeight="1"/>
+    <row r="787" ht="14.25" customHeight="1"/>
+    <row r="788" ht="14.25" customHeight="1"/>
+    <row r="789" ht="14.25" customHeight="1"/>
+    <row r="790" ht="14.25" customHeight="1"/>
+    <row r="791" ht="14.25" customHeight="1"/>
+    <row r="792" ht="14.25" customHeight="1"/>
+    <row r="793" ht="14.25" customHeight="1"/>
+    <row r="794" ht="14.25" customHeight="1"/>
+    <row r="795" ht="14.25" customHeight="1"/>
+    <row r="796" ht="14.25" customHeight="1"/>
+    <row r="797" ht="14.25" customHeight="1"/>
+    <row r="798" ht="14.25" customHeight="1"/>
+    <row r="799" ht="14.25" customHeight="1"/>
+    <row r="800" ht="14.25" customHeight="1"/>
+    <row r="801" ht="14.25" customHeight="1"/>
+    <row r="802" ht="14.25" customHeight="1"/>
+    <row r="803" ht="14.25" customHeight="1"/>
+    <row r="804" ht="14.25" customHeight="1"/>
+    <row r="805" ht="14.25" customHeight="1"/>
+    <row r="806" ht="14.25" customHeight="1"/>
+    <row r="807" ht="14.25" customHeight="1"/>
+    <row r="808" ht="14.25" customHeight="1"/>
+    <row r="809" ht="14.25" customHeight="1"/>
+    <row r="810" ht="14.25" customHeight="1"/>
+    <row r="811" ht="14.25" customHeight="1"/>
+    <row r="812" ht="14.25" customHeight="1"/>
+    <row r="813" ht="14.25" customHeight="1"/>
+    <row r="814" ht="14.25" customHeight="1"/>
+    <row r="815" ht="14.25" customHeight="1"/>
+    <row r="816" ht="14.25" customHeight="1"/>
+    <row r="817" ht="14.25" customHeight="1"/>
+    <row r="818" ht="14.25" customHeight="1"/>
+    <row r="819" ht="14.25" customHeight="1"/>
+    <row r="820" ht="14.25" customHeight="1"/>
+    <row r="821" ht="14.25" customHeight="1"/>
+    <row r="822" ht="14.25" customHeight="1"/>
+    <row r="823" ht="14.25" customHeight="1"/>
+    <row r="824" ht="14.25" customHeight="1"/>
+    <row r="825" ht="14.25" customHeight="1"/>
+    <row r="826" ht="14.25" customHeight="1"/>
+    <row r="827" ht="14.25" customHeight="1"/>
+    <row r="828" ht="14.25" customHeight="1"/>
+    <row r="829" ht="14.25" customHeight="1"/>
+    <row r="830" ht="14.25" customHeight="1"/>
+    <row r="831" ht="14.25" customHeight="1"/>
+    <row r="832" ht="14.25" customHeight="1"/>
+    <row r="833" ht="14.25" customHeight="1"/>
+    <row r="834" ht="14.25" customHeight="1"/>
+    <row r="835" ht="14.25" customHeight="1"/>
+    <row r="836" ht="14.25" customHeight="1"/>
+    <row r="837" ht="14.25" customHeight="1"/>
+    <row r="838" ht="14.25" customHeight="1"/>
+    <row r="839" ht="14.25" customHeight="1"/>
+    <row r="840" ht="14.25" customHeight="1"/>
+    <row r="841" ht="14.25" customHeight="1"/>
+    <row r="842" ht="14.25" customHeight="1"/>
+    <row r="843" ht="14.25" customHeight="1"/>
+    <row r="844" ht="14.25" customHeight="1"/>
+    <row r="845" ht="14.25" customHeight="1"/>
+    <row r="846" ht="14.25" customHeight="1"/>
+    <row r="847" ht="14.25" customHeight="1"/>
+    <row r="848" ht="14.25" customHeight="1"/>
+    <row r="849" ht="14.25" customHeight="1"/>
+    <row r="850" ht="14.25" customHeight="1"/>
+    <row r="851" ht="14.25" customHeight="1"/>
+    <row r="852" ht="14.25" customHeight="1"/>
+    <row r="853" ht="14.25" customHeight="1"/>
+    <row r="854" ht="14.25" customHeight="1"/>
+    <row r="855" ht="14.25" customHeight="1"/>
+    <row r="856" ht="14.25" customHeight="1"/>
+    <row r="857" ht="14.25" customHeight="1"/>
+    <row r="858" ht="14.25" customHeight="1"/>
+    <row r="859" ht="14.25" customHeight="1"/>
+    <row r="860" ht="14.25" customHeight="1"/>
+    <row r="861" ht="14.25" customHeight="1"/>
+    <row r="862" ht="14.25" customHeight="1"/>
+    <row r="863" ht="14.25" customHeight="1"/>
+    <row r="864" ht="14.25" customHeight="1"/>
+    <row r="865" ht="14.25" customHeight="1"/>
+    <row r="866" ht="14.25" customHeight="1"/>
+    <row r="867" ht="14.25" customHeight="1"/>
+    <row r="868" ht="14.25" customHeight="1"/>
+    <row r="869" ht="14.25" customHeight="1"/>
+    <row r="870" ht="14.25" customHeight="1"/>
+    <row r="871" ht="14.25" customHeight="1"/>
+    <row r="872" ht="14.25" customHeight="1"/>
+    <row r="873" ht="14.25" customHeight="1"/>
+    <row r="874" ht="14.25" customHeight="1"/>
+    <row r="875" ht="14.25" customHeight="1"/>
+    <row r="876" ht="14.25" customHeight="1"/>
+    <row r="877" ht="14.25" customHeight="1"/>
+    <row r="878" ht="14.25" customHeight="1"/>
+    <row r="879" ht="14.25" customHeight="1"/>
+    <row r="880" ht="14.25" customHeight="1"/>
+    <row r="881" ht="14.25" customHeight="1"/>
+    <row r="882" ht="14.25" customHeight="1"/>
+    <row r="883" ht="14.25" customHeight="1"/>
+    <row r="884" ht="14.25" customHeight="1"/>
+    <row r="885" ht="14.25" customHeight="1"/>
+    <row r="886" ht="14.25" customHeight="1"/>
+    <row r="887" ht="14.25" customHeight="1"/>
+    <row r="888" ht="14.25" customHeight="1"/>
+    <row r="889" ht="14.25" customHeight="1"/>
+    <row r="890" ht="14.25" customHeight="1"/>
+    <row r="891" ht="14.25" customHeight="1"/>
+    <row r="892" ht="14.25" customHeight="1"/>
+    <row r="893" ht="14.25" customHeight="1"/>
+    <row r="894" ht="14.25" customHeight="1"/>
+    <row r="895" ht="14.25" customHeight="1"/>
+    <row r="896" ht="14.25" customHeight="1"/>
+    <row r="897" ht="14.25" customHeight="1"/>
+    <row r="898" ht="14.25" customHeight="1"/>
+    <row r="899" ht="14.25" customHeight="1"/>
+    <row r="900" ht="14.25" customHeight="1"/>
+    <row r="901" ht="14.25" customHeight="1"/>
+    <row r="902" ht="14.25" customHeight="1"/>
+    <row r="903" ht="14.25" customHeight="1"/>
+    <row r="904" ht="14.25" customHeight="1"/>
+    <row r="905" ht="14.25" customHeight="1"/>
+    <row r="906" ht="14.25" customHeight="1"/>
+    <row r="907" ht="14.25" customHeight="1"/>
+    <row r="908" ht="14.25" customHeight="1"/>
+    <row r="909" ht="14.25" customHeight="1"/>
+    <row r="910" ht="14.25" customHeight="1"/>
+    <row r="911" ht="14.25" customHeight="1"/>
+    <row r="912" ht="14.25" customHeight="1"/>
+    <row r="913" ht="14.25" customHeight="1"/>
+    <row r="914" ht="14.25" customHeight="1"/>
+    <row r="915" ht="14.25" customHeight="1"/>
+    <row r="916" ht="14.25" customHeight="1"/>
+    <row r="917" ht="14.25" customHeight="1"/>
+    <row r="918" ht="14.25" customHeight="1"/>
+    <row r="919" ht="14.25" customHeight="1"/>
+    <row r="920" ht="14.25" customHeight="1"/>
+    <row r="921" ht="14.25" customHeight="1"/>
+    <row r="922" ht="14.25" customHeight="1"/>
+    <row r="923" ht="14.25" customHeight="1"/>
+    <row r="924" ht="14.25" customHeight="1"/>
+    <row r="925" ht="14.25" customHeight="1"/>
+    <row r="926" ht="14.25" customHeight="1"/>
+    <row r="927" ht="14.25" customHeight="1"/>
+    <row r="928" ht="14.25" customHeight="1"/>
+    <row r="929" ht="14.25" customHeight="1"/>
+    <row r="930" ht="14.25" customHeight="1"/>
+    <row r="931" ht="14.25" customHeight="1"/>
+    <row r="932" ht="14.25" customHeight="1"/>
+    <row r="933" ht="14.25" customHeight="1"/>
+    <row r="934" ht="14.25" customHeight="1"/>
+    <row r="935" ht="14.25" customHeight="1"/>
+    <row r="936" ht="14.25" customHeight="1"/>
+    <row r="937" ht="14.25" customHeight="1"/>
+    <row r="938" ht="14.25" customHeight="1"/>
+    <row r="939" ht="14.25" customHeight="1"/>
+    <row r="940" ht="14.25" customHeight="1"/>
+    <row r="941" ht="14.25" customHeight="1"/>
+    <row r="942" ht="14.25" customHeight="1"/>
+    <row r="943" ht="14.25" customHeight="1"/>
+    <row r="944" ht="14.25" customHeight="1"/>
+    <row r="945" ht="14.25" customHeight="1"/>
+    <row r="946" ht="14.25" customHeight="1"/>
+    <row r="947" ht="14.25" customHeight="1"/>
+    <row r="948" ht="14.25" customHeight="1"/>
+    <row r="949" ht="14.25" customHeight="1"/>
+    <row r="950" ht="14.25" customHeight="1"/>
+    <row r="951" ht="14.25" customHeight="1"/>
+    <row r="952" ht="14.25" customHeight="1"/>
+    <row r="953" ht="14.25" customHeight="1"/>
+    <row r="954" ht="14.25" customHeight="1"/>
+    <row r="955" ht="14.25" customHeight="1"/>
+    <row r="956" ht="14.25" customHeight="1"/>
+    <row r="957" ht="14.25" customHeight="1"/>
+    <row r="958" ht="14.25" customHeight="1"/>
+    <row r="959" ht="14.25" customHeight="1"/>
+    <row r="960" ht="14.25" customHeight="1"/>
+    <row r="961" ht="14.25" customHeight="1"/>
+    <row r="962" ht="14.25" customHeight="1"/>
+    <row r="963" ht="14.25" customHeight="1"/>
+    <row r="964" ht="14.25" customHeight="1"/>
+    <row r="965" ht="14.25" customHeight="1"/>
+    <row r="966" ht="14.25" customHeight="1"/>
+    <row r="967" ht="14.25" customHeight="1"/>
+    <row r="968" ht="14.25" customHeight="1"/>
+    <row r="969" ht="14.25" customHeight="1"/>
+    <row r="970" ht="14.25" customHeight="1"/>
+    <row r="971" ht="14.25" customHeight="1"/>
+    <row r="972" ht="14.25" customHeight="1"/>
+    <row r="973" ht="14.25" customHeight="1"/>
+    <row r="974" ht="14.25" customHeight="1"/>
+    <row r="975" ht="14.25" customHeight="1"/>
+    <row r="976" ht="14.25" customHeight="1"/>
+    <row r="977" ht="14.25" customHeight="1"/>
+    <row r="978" ht="14.25" customHeight="1"/>
+    <row r="979" ht="14.25" customHeight="1"/>
+    <row r="980" ht="14.25" customHeight="1"/>
+    <row r="981" ht="14.25" customHeight="1"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D4:D5 D10:D11 D2" xr:uid="{EDBC99A1-A261-4DB3-AB95-B6295D7B1159}">
-      <formula1>"Texte,Bool,Entier"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{6E08AB50-8F1B-430C-80E8-3DF93C78C59F}">
+      <formula1>"Texte,Bool,Entier,Login,Pwd"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6508,7 +6430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -6803,7 +6725,7 @@
         <v>45</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D21" s="7">
         <v>1</v>
@@ -6825,13 +6747,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
@@ -6839,13 +6761,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D25" s="7">
         <v>0</v>
@@ -6853,13 +6775,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -6875,8 +6797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8340,8 +8262,8 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10 D14:D15 D17:D18 D23:D24 D20:D21 D6:D7" xr:uid="{EAD0B869-C39C-4665-BB02-4D2BB2300FFD}">
-      <formula1>"Texte,Bool,Entier"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D1048576 D2:D13" xr:uid="{4A82DEC5-6073-474E-9CB9-DD21A09A9CB7}">
+      <formula1>"Texte,Bool,Entier,Login,Pwd"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Initialisation Settings OK :-)
</commit_message>
<xml_diff>
--- a/Template/Data/Config_REFC.xlsx
+++ b/Template/Data/Config_REFC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renau\GitHub\RPA_Template-RHENRY\Template\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E71133-BD7A-4528-9F54-FB36FF4D5517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB11024B-1DEE-40FA-A9E4-BCF5E5C64711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="PrePROD" sheetId="4" r:id="rId3"/>
     <sheet name="PROD" sheetId="1" r:id="rId4"/>
     <sheet name="Core-Constants" sheetId="7" r:id="rId5"/>
-    <sheet name="Str" sheetId="8" r:id="rId6"/>
+    <sheet name="Core-Assets" sheetId="8" r:id="rId6"/>
     <sheet name="Constants" sheetId="2" r:id="rId7"/>
     <sheet name="Assets" sheetId="3" r:id="rId8"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -238,9 +238,6 @@
     <t>Port</t>
   </si>
   <si>
-    <t>Credential</t>
-  </si>
-  <si>
     <t>LogDB_NOSQL</t>
   </si>
   <si>
@@ -343,21 +340,9 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Email_CredentialSMTP_Login</t>
-  </si>
-  <si>
     <t>Pwd</t>
   </si>
   <si>
-    <t>Email_CredentialSMTP_Pwd</t>
-  </si>
-  <si>
-    <t>LogDB_NOSQL_Credential_Login</t>
-  </si>
-  <si>
-    <t>LogDB_NOSQL_Credential_Pwd</t>
-  </si>
-  <si>
     <t>IS Paterne</t>
   </si>
   <si>
@@ -409,7 +394,19 @@
     <t>https://github.com/renaudfractale/</t>
   </si>
   <si>
-    <t>Data\{{Projet}}\{{Env}}</t>
+    <t>Data\Output\{{Env}}</t>
+  </si>
+  <si>
+    <t>LogDB_NOSQL_Credential</t>
+  </si>
+  <si>
+    <t>Credential_Login</t>
+  </si>
+  <si>
+    <t>Credential_Pwd</t>
+  </si>
+  <si>
+    <t>Email_CredentialSMTP</t>
   </si>
 </sst>
 </file>
@@ -468,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -506,6 +503,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -825,7 +825,7 @@
   <dimension ref="A1:AA998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -879,10 +879,10 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C2" s="12">
         <v>2</v>
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -1931,7 +1931,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1960,10 +1960,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -3012,7 +3012,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -3041,10 +3041,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -3053,7 +3053,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -4092,7 +4092,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -4121,10 +4121,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -4133,7 +4133,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -5147,10 +5147,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2667E7E-E5B4-45AB-A62C-C441EF002CA9}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5161,7 +5161,7 @@
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -5171,11 +5171,14 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -5183,11 +5186,13 @@
         <v>47</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -5197,39 +5202,50 @@
       <c r="C3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
         <v>72</v>
       </c>
-      <c r="C5" t="s">
-        <v>73</v>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>108</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5242,7 +5258,7 @@
   <dimension ref="A1:AA981"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D1048576"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5269,13 +5285,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>4</v>
@@ -5303,13 +5319,13 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>52</v>
@@ -5326,13 +5342,13 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>52</v>
@@ -5353,13 +5369,13 @@
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>52</v>
@@ -5376,13 +5392,13 @@
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>52</v>
@@ -5400,13 +5416,13 @@
     <row r="7" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:27" ht="14.25" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>52</v>
@@ -5423,13 +5439,13 @@
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>52</v>
@@ -6430,8 +6446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -6456,7 +6472,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>3</v>
@@ -6725,21 +6741,24 @@
         <v>45</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D21" s="7">
         <v>1</v>
       </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>99</v>
       </c>
       <c r="D23" s="7">
         <v>0</v>
@@ -6747,13 +6766,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
@@ -6761,13 +6780,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D25" s="7">
         <v>0</v>
@@ -6775,13 +6794,16 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6797,13 +6819,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="34" customWidth="1"/>
@@ -6822,13 +6845,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -6862,10 +6885,10 @@
         <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>58</v>
@@ -6885,10 +6908,10 @@
         <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>58</v>
@@ -6908,10 +6931,10 @@
         <v>55</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>58</v>
@@ -6928,13 +6951,13 @@
         <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>58</v>
@@ -6957,7 +6980,7 @@
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>56</v>
@@ -6980,16 +7003,16 @@
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>58</v>
@@ -7003,16 +7026,16 @@
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>58</v>
@@ -7026,7 +7049,7 @@
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
         <v>65</v>
@@ -7050,16 +7073,16 @@
     <row r="11" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:27" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>58</v>
@@ -7073,16 +7096,16 @@
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>58</v>
@@ -7096,13 +7119,13 @@
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
         <v>67</v>
-      </c>
-      <c r="B14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>52</v>
@@ -7119,16 +7142,16 @@
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
         <v>74</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>58</v>
@@ -7143,16 +7166,16 @@
     <row r="16" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:7" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>58</v>
@@ -7166,13 +7189,13 @@
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
         <v>79</v>
-      </c>
-      <c r="B18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" t="s">
-        <v>80</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>52</v>
@@ -7190,19 +7213,19 @@
     <row r="19" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" t="s">
         <v>89</v>
-      </c>
-      <c r="B20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" t="s">
-        <v>90</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
@@ -7213,19 +7236,19 @@
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
@@ -7240,48 +7263,48 @@
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
       </c>
-      <c r="G23" t="s">
-        <v>53</v>
+      <c r="G23" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
       </c>
-      <c r="G24" t="s">
-        <v>53</v>
+      <c r="G24" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1"/>
@@ -8262,7 +8285,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D1048576 D2:D13" xr:uid="{4A82DEC5-6073-474E-9CB9-DD21A09A9CB7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{4A82DEC5-6073-474E-9CB9-DD21A09A9CB7}">
       <formula1>"Texte,Bool,Entier,Login,Pwd"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Dispatcher en cours de réalisation
</commit_message>
<xml_diff>
--- a/Template/Data/Config_REFC.xlsx
+++ b/Template/Data/Config_REFC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renau\GitHub\RPA_Template-RHENRY\Template\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB11024B-1DEE-40FA-A9E4-BCF5E5C64711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE3A30F-7599-4059-A147-F3A588663A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>Email_CredentialSMTP</t>
+  </si>
+  <si>
+    <t>RAZ</t>
   </si>
 </sst>
 </file>
@@ -6444,10 +6447,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -6806,6 +6809,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -6819,7 +6836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mise en place du mail Recap ?
</commit_message>
<xml_diff>
--- a/Template/Data/Config_REFC.xlsx
+++ b/Template/Data/Config_REFC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renau\GitHub\RPA_Template-RHENRY\Template\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C11EFA-33A4-452D-844B-F211CFA88ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA3C8C-74DA-42BB-99AB-43E4903121FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="128">
   <si>
     <t>Name</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>CCEmailError</t>
+  </si>
+  <si>
+    <t>DestinataireEmailRecap</t>
+  </si>
+  <si>
+    <t>CCEmailRecap</t>
   </si>
 </sst>
 </file>
@@ -5159,7 +5165,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5264,13 +5270,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BC9249-B8A7-4BE9-B73B-28D49C06D735}">
-  <dimension ref="A1:AA981"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
@@ -5283,7 +5289,7 @@
     <col min="28" max="16384" width="14.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="14.25" customHeight="1">
+    <row r="1" spans="1:27" ht="18.75">
       <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
@@ -5326,7 +5332,7 @@
       <c r="Z1" s="6"/>
       <c r="AA1" s="6"/>
     </row>
-    <row r="2" spans="1:27" ht="14.25" customHeight="1">
+    <row r="2" spans="1:27">
       <c r="A2" s="7" t="s">
         <v>88</v>
       </c>
@@ -5349,7 +5355,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="14.25" customHeight="1">
+    <row r="3" spans="1:27">
       <c r="A3" s="7" t="s">
         <v>88</v>
       </c>
@@ -5372,11 +5378,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="14.25" customHeight="1">
+    <row r="4" spans="1:27">
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:27" ht="14.25" customHeight="1">
+    <row r="5" spans="1:27">
       <c r="A5" s="7" t="s">
         <v>88</v>
       </c>
@@ -5399,7 +5405,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="14.25" customHeight="1">
+    <row r="6" spans="1:27">
       <c r="A6" s="7" t="s">
         <v>88</v>
       </c>
@@ -5422,8 +5428,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:27" ht="14.25" customHeight="1">
+    <row r="8" spans="1:27">
       <c r="A8" s="7" t="s">
         <v>103</v>
       </c>
@@ -5446,7 +5451,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1">
+    <row r="9" spans="1:27">
       <c r="A9" s="7" t="s">
         <v>103</v>
       </c>
@@ -5469,978 +5474,6 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{6E08AB50-8F1B-430C-80E8-3DF93C78C59F}">
@@ -6839,8 +5872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:G30"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7333,10 +6366,10 @@
         <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>52</v>
@@ -7356,10 +6389,10 @@
         <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Edit Set Transaction Statuts
</commit_message>
<xml_diff>
--- a/Template/Data/Config_REFC.xlsx
+++ b/Template/Data/Config_REFC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renau\GitHub\RPA_Template-RHENRY\Template\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA3C8C-74DA-42BB-99AB-43E4903121FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A139E3-1750-4090-AB22-BDBDAFD46A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -172,9 +172,6 @@
     <t>FolderRecap</t>
   </si>
   <si>
-    <t>Data\Recap</t>
-  </si>
-  <si>
     <t>FolderOut</t>
   </si>
   <si>
@@ -422,6 +419,12 @@
   </si>
   <si>
     <t>CCEmailRecap</t>
+  </si>
+  <si>
+    <t>With_Monkey</t>
+  </si>
+  <si>
+    <t>Data\Recap\{{Env}}</t>
   </si>
 </sst>
 </file>
@@ -840,7 +843,7 @@
   <dimension ref="A1:AA998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -865,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -894,10 +897,10 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>113</v>
       </c>
       <c r="C2" s="12">
         <v>2</v>
@@ -906,13 +909,22 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
+      <c r="A3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:27">
@@ -1946,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1975,10 +1987,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>113</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -1987,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -3027,7 +3039,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -3056,10 +3068,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>113</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -3068,7 +3080,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -4107,7 +4119,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -4136,10 +4148,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>113</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -4148,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -5187,7 +5199,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -5195,13 +5207,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -5209,13 +5221,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -5223,13 +5235,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -5237,13 +5249,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
         <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>72</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -5251,13 +5263,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
         <v>107</v>
-      </c>
-      <c r="C6" t="s">
-        <v>108</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -5300,13 +5312,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>4</v>
@@ -5334,48 +5346,48 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>89</v>
-      </c>
       <c r="D2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="9">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:27">
       <c r="A3" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="9">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -5384,94 +5396,94 @@
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="9">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="9">
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:27">
       <c r="A9" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="D9" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -5486,10 +5498,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA28"/>
+  <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -5514,7 +5526,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>3</v>
@@ -5544,7 +5556,7 @@
     </row>
     <row r="2" spans="1:27" ht="60">
       <c r="A2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>5</v>
@@ -5561,10 +5573,10 @@
     </row>
     <row r="3" spans="1:27" ht="60">
       <c r="A3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="9">
         <v>0</v>
@@ -5573,7 +5585,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -5729,33 +5741,33 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
+      <c r="A17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0</v>
-      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="7">
         <v>0</v>
@@ -5763,13 +5775,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D20" s="7">
         <v>0</v>
@@ -5777,44 +5789,44 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D21" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="C22" s="16"/>
+      <c r="A22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
@@ -5822,43 +5834,57 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="D25" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="7">
+    <row r="26" spans="1:4">
+      <c r="A26" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="D28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="7">
         <v>0</v>
       </c>
     </row>
@@ -5872,7 +5898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -5898,13 +5924,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -5932,94 +5958,94 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="4">
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1">
@@ -6033,281 +6059,281 @@
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
         <v>120</v>
       </c>
-      <c r="C9" t="s">
-        <v>121</v>
-      </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" s="4">
         <v>0</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:27" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" s="4">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
         <v>66</v>
       </c>
-      <c r="B14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" s="4">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" s="4">
         <v>0</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:7" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F17" s="4">
         <v>0</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
         <v>78</v>
       </c>
-      <c r="B18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
         <v>88</v>
       </c>
-      <c r="B20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" t="s">
-        <v>89</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1">
@@ -6316,142 +6342,142 @@
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:7" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:7" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
A finir: Propager DicoOutput
</commit_message>
<xml_diff>
--- a/Template/Data/Config_REFC.xlsx
+++ b/Template/Data/Config_REFC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renau\GitHub\RPA_Template-RHENRY\Template\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0970E982-399B-40AA-9ADF-17F58C34E3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B952962-B078-402D-9969-1D0710560547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="2370" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="2370" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV" sheetId="6" r:id="rId1"/>
@@ -5275,7 +5275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BC9249-B8A7-4BE9-B73B-28D49C06D735}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -5491,8 +5491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
OK pour communiquer le projet
</commit_message>
<xml_diff>
--- a/Template/Data/Config_REFC.xlsx
+++ b/Template/Data/Config_REFC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renau\GitHub\RPA_Template-RHENRY\Template\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C607534C-E58B-402D-9A0C-8037C7E00674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3C305A-8872-4DCD-98B2-657D30D860E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -148,277 +148,274 @@
     <t>NB_Monkey</t>
   </si>
   <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>FolderArchive</t>
+  </si>
+  <si>
+    <t>Data\Archive</t>
+  </si>
+  <si>
+    <t>FolderWorking</t>
+  </si>
+  <si>
+    <t>Data\Temp</t>
+  </si>
+  <si>
+    <t>Recap</t>
+  </si>
+  <si>
+    <t>FolderRecap</t>
+  </si>
+  <si>
+    <t>FolderOut</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Processus</t>
+  </si>
+  <si>
+    <t>Projet</t>
+  </si>
+  <si>
+    <t>RPA0000</t>
+  </si>
+  <si>
+    <t>Orchestrator</t>
+  </si>
+  <si>
+    <t>client_id</t>
+  </si>
+  <si>
+    <t>Texte</t>
+  </si>
+  <si>
+    <t>Facultatif</t>
+  </si>
+  <si>
+    <t>refresh_token</t>
+  </si>
+  <si>
+    <t>TenantName</t>
+  </si>
+  <si>
+    <t>ServerSMTP</t>
+  </si>
+  <si>
+    <t>Obligatoire</t>
+  </si>
+  <si>
+    <t>CONFIG</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>TryErrors</t>
+  </si>
+  <si>
+    <t>Email_Port</t>
+  </si>
+  <si>
+    <t>Email_ServeurSMTP</t>
+  </si>
+  <si>
+    <t>Entier</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>LogDB_NOSQL</t>
+  </si>
+  <si>
+    <t>LogDB_NOSQL_URL</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Unite</t>
+  </si>
+  <si>
+    <t>TemplateFolder</t>
+  </si>
+  <si>
+    <t>Pays</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>IsActif</t>
+  </si>
+  <si>
+    <t>LogDB_NOSQL_Actif</t>
+  </si>
+  <si>
+    <t>Bool</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>LogTxt_Actif</t>
+  </si>
+  <si>
+    <t>LogTxt</t>
+  </si>
+  <si>
+    <t>LogTxt_PathFolderBase</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Orchestrator_client_id</t>
+  </si>
+  <si>
+    <t>Orchestrator_refresh_token</t>
+  </si>
+  <si>
+    <t>Orchestrator_TenantName</t>
+  </si>
+  <si>
+    <t>AccountLogicalName</t>
+  </si>
+  <si>
+    <t>Orchestrator_AccountLogicalName</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Template 1.00 REF Custom</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Email_NameError</t>
+  </si>
+  <si>
+    <t>Email_EmailError</t>
+  </si>
+  <si>
+    <t>NameError</t>
+  </si>
+  <si>
+    <t>EmailError</t>
+  </si>
+  <si>
+    <t>NameRecap</t>
+  </si>
+  <si>
+    <t>EmaiRecap</t>
+  </si>
+  <si>
+    <t>Email_NameRecap</t>
+  </si>
+  <si>
+    <t>Email_EmailRecap</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Pwd</t>
+  </si>
+  <si>
+    <t>IS Paterne</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>TemplateQlist</t>
+  </si>
+  <si>
+    <t>RégionDuMonde</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Performer</t>
+  </si>
+  <si>
+    <t>With</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Dispatcher</t>
+  </si>
+  <si>
+    <t>NbDepot</t>
+  </si>
+  <si>
+    <t>Nombre de dépots téléchargé</t>
+  </si>
+  <si>
+    <t>SiteWeb</t>
+  </si>
+  <si>
+    <t>Data\Output\{{Env}}</t>
+  </si>
+  <si>
+    <t>LogDB_NOSQL_Credential</t>
+  </si>
+  <si>
+    <t>Credential_Login</t>
+  </si>
+  <si>
+    <t>Credential_Pwd</t>
+  </si>
+  <si>
+    <t>Email_CredentialSMTP</t>
+  </si>
+  <si>
+    <t>RAZ</t>
+  </si>
+  <si>
+    <t>https://github.com/renaudfractale?tab=repositories</t>
+  </si>
+  <si>
+    <t>DestinataireEmailError</t>
+  </si>
+  <si>
+    <t>CCEmailError</t>
+  </si>
+  <si>
+    <t>DestinataireEmailRecap</t>
+  </si>
+  <si>
+    <t>CCEmailRecap</t>
+  </si>
+  <si>
+    <t>With_Monkey</t>
+  </si>
+  <si>
+    <t>Data\Recap\{{Env}}</t>
+  </si>
+  <si>
+    <t>QListe</t>
+  </si>
+  <si>
+    <t>EmailRecap</t>
+  </si>
+  <si>
     <t>33/100</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>FolderArchive</t>
-  </si>
-  <si>
-    <t>Data\Archive</t>
-  </si>
-  <si>
-    <t>FolderWorking</t>
-  </si>
-  <si>
-    <t>Data\Temp</t>
-  </si>
-  <si>
-    <t>Recap</t>
-  </si>
-  <si>
-    <t>FolderRecap</t>
-  </si>
-  <si>
-    <t>FolderOut</t>
-  </si>
-  <si>
-    <t>Core</t>
-  </si>
-  <si>
-    <t>Processus</t>
-  </si>
-  <si>
-    <t>Projet</t>
-  </si>
-  <si>
-    <t>RPA0000</t>
-  </si>
-  <si>
-    <t>Orchestrator</t>
-  </si>
-  <si>
-    <t>client_id</t>
-  </si>
-  <si>
-    <t>Texte</t>
-  </si>
-  <si>
-    <t>Facultatif</t>
-  </si>
-  <si>
-    <t>refresh_token</t>
-  </si>
-  <si>
-    <t>TenantName</t>
-  </si>
-  <si>
-    <t>ServerSMTP</t>
-  </si>
-  <si>
-    <t>Obligatoire</t>
-  </si>
-  <si>
-    <t>CONFIG</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>TryErrors</t>
-  </si>
-  <si>
-    <t>Email_Port</t>
-  </si>
-  <si>
-    <t>Email_ServeurSMTP</t>
-  </si>
-  <si>
-    <t>Entier</t>
-  </si>
-  <si>
-    <t>Port</t>
-  </si>
-  <si>
-    <t>LogDB_NOSQL</t>
-  </si>
-  <si>
-    <t>LogDB_NOSQL_URL</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>Unite</t>
-  </si>
-  <si>
-    <t>TemplateFolder</t>
-  </si>
-  <si>
-    <t>Pays</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>IsActif</t>
-  </si>
-  <si>
-    <t>LogDB_NOSQL_Actif</t>
-  </si>
-  <si>
-    <t>Bool</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>LogTxt_Actif</t>
-  </si>
-  <si>
-    <t>LogTxt</t>
-  </si>
-  <si>
-    <t>LogTxt_PathFolderBase</t>
-  </si>
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>Orchestrator_client_id</t>
-  </si>
-  <si>
-    <t>Orchestrator_refresh_token</t>
-  </si>
-  <si>
-    <t>Orchestrator_TenantName</t>
-  </si>
-  <si>
-    <t>AccountLogicalName</t>
-  </si>
-  <si>
-    <t>Orchestrator_AccountLogicalName</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>Template 1.00 REF Custom</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Email_NameError</t>
-  </si>
-  <si>
-    <t>Email_EmailError</t>
-  </si>
-  <si>
-    <t>NameError</t>
-  </si>
-  <si>
-    <t>EmailError</t>
-  </si>
-  <si>
-    <t>NameRecap</t>
-  </si>
-  <si>
-    <t>EmaiRecap</t>
-  </si>
-  <si>
-    <t>Email_NameRecap</t>
-  </si>
-  <si>
-    <t>Email_EmailRecap</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Pwd</t>
-  </si>
-  <si>
-    <t>IS Paterne</t>
-  </si>
-  <si>
-    <t>Folder</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>TemplateQlist</t>
-  </si>
-  <si>
-    <t>RégionDuMonde</t>
-  </si>
-  <si>
-    <t>Europe</t>
-  </si>
-  <si>
-    <t>Performer</t>
-  </si>
-  <si>
-    <t>With</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>Dispatcher</t>
-  </si>
-  <si>
-    <t>NbDepot</t>
-  </si>
-  <si>
-    <t>Nombre de dépots téléchargé</t>
-  </si>
-  <si>
-    <t>SiteWeb</t>
-  </si>
-  <si>
-    <t>Data\Output\{{Env}}</t>
-  </si>
-  <si>
-    <t>LogDB_NOSQL_Credential</t>
-  </si>
-  <si>
-    <t>Credential_Login</t>
-  </si>
-  <si>
-    <t>Credential_Pwd</t>
-  </si>
-  <si>
-    <t>Email_CredentialSMTP</t>
-  </si>
-  <si>
-    <t>RAZ</t>
-  </si>
-  <si>
-    <t>https://github.com/renaudfractale?tab=repositories</t>
-  </si>
-  <si>
-    <t>DestinataireEmailError</t>
-  </si>
-  <si>
-    <t>CCEmailError</t>
-  </si>
-  <si>
-    <t>DestinataireEmailRecap</t>
-  </si>
-  <si>
-    <t>CCEmailRecap</t>
-  </si>
-  <si>
-    <t>With_Monkey</t>
-  </si>
-  <si>
-    <t>Data\Recap\{{Env}}</t>
-  </si>
-  <si>
-    <t>QListe</t>
-  </si>
-  <si>
-    <t>EmailRecap</t>
   </si>
 </sst>
 </file>
@@ -862,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -891,10 +888,10 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="12">
         <v>2</v>
@@ -903,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -911,10 +908,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" s="13">
         <v>0</v>
@@ -1952,7 +1949,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1981,10 +1978,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -1993,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -3033,7 +3030,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -3062,10 +3059,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -3074,7 +3071,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -4113,7 +4110,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -4142,10 +4139,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -4154,7 +4151,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -5193,7 +5190,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -5201,13 +5198,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -5215,13 +5212,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -5229,13 +5226,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -5243,13 +5240,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
         <v>70</v>
-      </c>
-      <c r="C5" t="s">
-        <v>71</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -5257,13 +5254,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -5306,13 +5303,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>4</v>
@@ -5340,48 +5337,48 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="D2" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="9">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:27">
       <c r="A3" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="9">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -5390,94 +5387,94 @@
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="9">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="9">
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:27">
       <c r="A9" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -5494,8 +5491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -5520,7 +5517,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>3</v>
@@ -5550,7 +5547,7 @@
     </row>
     <row r="2" spans="1:27" ht="60">
       <c r="A2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>5</v>
@@ -5567,10 +5564,10 @@
     </row>
     <row r="3" spans="1:27" ht="60">
       <c r="A3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="9">
         <v>0</v>
@@ -5579,7 +5576,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -5682,6 +5679,9 @@
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
       <c r="E11" s="8" t="s">
         <v>23</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>35</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="D16" s="7">
         <v>0</v>
@@ -5739,10 +5739,10 @@
         <v>34</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D17" s="13">
         <v>0</v>
@@ -5755,13 +5755,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="D19" s="7">
         <v>0</v>
@@ -5769,13 +5769,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="D20" s="7">
         <v>0</v>
@@ -5783,13 +5783,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="C21" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D21" s="7">
         <v>1</v>
@@ -5797,13 +5797,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D22" s="7">
         <v>1</v>
@@ -5814,13 +5814,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
@@ -5828,13 +5828,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="D25" s="7">
         <v>0</v>
@@ -5842,13 +5842,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D26" s="7">
         <v>0</v>
@@ -5856,13 +5856,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D28" s="7">
         <v>0</v>
@@ -5870,13 +5870,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D29" s="7">
         <v>0</v>
@@ -5918,13 +5918,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -5952,94 +5952,94 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="4">
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1">
@@ -6053,281 +6053,281 @@
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
         <v>114</v>
       </c>
-      <c r="C8" t="s">
-        <v>116</v>
-      </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10" s="4">
         <v>0</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:27" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="4">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" s="4">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
         <v>72</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="4">
         <v>0</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:7" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="4">
         <v>0</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
         <v>77</v>
       </c>
-      <c r="B18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" t="s">
-        <v>78</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
         <v>87</v>
       </c>
-      <c r="B20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" t="s">
-        <v>88</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1">
@@ -6336,142 +6336,142 @@
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:7" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:7" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.25" customHeight="1"/>

</xml_diff>